<commit_message>
3sum and 4sum solved finally
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827C24E1-99CE-4F82-8765-2C8DE29773F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63AAC3C-D031-499C-8CFF-52F85A7701ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1514,8 +1514,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="111" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1675,7 +1675,7 @@
       <c r="C14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="29"/>
       <c r="G14" s="10" t="s">
         <v>13</v>
       </c>
@@ -1720,7 +1720,7 @@
       <c r="C18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="27"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1733,7 +1733,7 @@
       <c r="C19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="27"/>
+      <c r="D19" s="29"/>
       <c r="F19" s="10" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
string 4 question solved
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63AAC3C-D031-499C-8CFF-52F85A7701ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984518E0-14BC-4A25-B05D-E00837668C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1514,15 +1514,15 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.88671875" customWidth="1"/>
+    <col min="3" max="3" width="115.6640625" customWidth="1"/>
     <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
@@ -1902,7 +1902,7 @@
       <c r="C37" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="27"/>
+      <c r="D37" s="29"/>
       <c r="H37" s="10" t="s">
         <v>13</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="C38" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="27"/>
+      <c r="D38" s="29"/>
     </row>
     <row r="39" spans="2:8" ht="13.2">
       <c r="B39" s="8" t="s">
@@ -1923,7 +1923,7 @@
       <c r="C39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="27"/>
+      <c r="D39" s="29"/>
       <c r="H39" s="10" t="s">
         <v>13</v>
       </c>
@@ -1935,7 +1935,7 @@
       <c r="C40" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="27"/>
+      <c r="D40" s="29"/>
     </row>
     <row r="41" spans="2:8" ht="13.2">
       <c r="B41" s="8" t="s">
@@ -2008,7 +2008,7 @@
       <c r="C46" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="27"/>
+      <c r="D46" s="29"/>
       <c r="E46" s="10" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
solved 2 hard questions of string
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78003D1-5F2B-4FEC-AC4C-C35479C145CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC416B5E-FCD6-442B-B6F6-2E1B195D6C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1515,14 +1515,14 @@
   <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="93" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.21875" customWidth="1"/>
+    <col min="3" max="3" width="119.44140625" customWidth="1"/>
     <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
@@ -2062,7 +2062,7 @@
       <c r="C51" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="27"/>
+      <c r="D51" s="29"/>
       <c r="F51" s="11" t="s">
         <v>13</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="C52" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="27"/>
+      <c r="D52" s="29"/>
     </row>
     <row r="53" spans="2:8" ht="13.2">
       <c r="B53" s="8" t="s">

</xml_diff>

<commit_message>
1 medium question solved
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC416B5E-FCD6-442B-B6F6-2E1B195D6C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28C9AF9-2A50-4F6C-939D-052D5277E295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1514,8 +1514,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1959,7 +1959,7 @@
       <c r="C42" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="27"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="10" t="s">
         <v>13</v>
       </c>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="58" spans="2:8" ht="13.2">
       <c r="B58" s="6"/>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D58" s="27"/>

</xml_diff>

<commit_message>
7 easy mathematical question solved
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28C9AF9-2A50-4F6C-939D-052D5277E295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2469A5C-F688-48E6-8908-5E5AE0BBC17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1237,7 +1237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1271,7 +1271,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1514,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1580,7 +1579,7 @@
       <c r="C6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="26"/>
       <c r="I6" s="10" t="s">
         <v>13</v>
       </c>
@@ -1592,7 +1591,7 @@
       <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="10" t="s">
         <v>13</v>
       </c>
@@ -1610,7 +1609,7 @@
       <c r="C8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="10" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1621,7 @@
       <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="29"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:9" ht="13.2">
@@ -1632,7 +1631,7 @@
       <c r="C10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="29"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="10" t="s">
         <v>13</v>
       </c>
@@ -1644,7 +1643,7 @@
       <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="5"/>
       <c r="H11" s="10" t="s">
         <v>13</v>
@@ -1657,7 +1656,7 @@
       <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="29"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:9" ht="13.2">
       <c r="B13" s="8" t="s">
@@ -1666,7 +1665,7 @@
       <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="29"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:9" ht="13.2">
       <c r="B14" s="8" t="s">
@@ -1675,7 +1674,7 @@
       <c r="C14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="28"/>
       <c r="G14" s="10" t="s">
         <v>13</v>
       </c>
@@ -1687,7 +1686,7 @@
       <c r="C15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="27"/>
+      <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:9" ht="13.2">
       <c r="B16" s="8" t="s">
@@ -1696,7 +1695,7 @@
       <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="28"/>
       <c r="I16" s="10" t="s">
         <v>13</v>
       </c>
@@ -1708,7 +1707,7 @@
       <c r="C17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="27"/>
+      <c r="D17" s="26"/>
       <c r="F17" s="10" t="s">
         <v>13</v>
       </c>
@@ -1720,7 +1719,7 @@
       <c r="C18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="29"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1733,7 +1732,7 @@
       <c r="C19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="28"/>
       <c r="F19" s="10" t="s">
         <v>13</v>
       </c>
@@ -1745,7 +1744,7 @@
       <c r="C20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="27"/>
+      <c r="D20" s="26"/>
       <c r="F20" s="10" t="s">
         <v>13</v>
       </c>
@@ -1757,7 +1756,7 @@
       <c r="C21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="27"/>
+      <c r="D21" s="26"/>
       <c r="I21" s="10" t="s">
         <v>13</v>
       </c>
@@ -1769,7 +1768,7 @@
       <c r="C22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="28"/>
     </row>
     <row r="23" spans="2:9" ht="13.2">
       <c r="B23" s="8" t="s">
@@ -1778,7 +1777,7 @@
       <c r="C23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="2:9" ht="13.2">
       <c r="B24" s="8" t="s">
@@ -1787,7 +1786,7 @@
       <c r="C24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="2:9" ht="13.2">
       <c r="B25" s="8" t="s">
@@ -1796,7 +1795,7 @@
       <c r="C25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="2:9" ht="13.2">
       <c r="B26" s="8" t="s">
@@ -1805,7 +1804,7 @@
       <c r="C26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="27"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="2:9" ht="13.2">
       <c r="B27" s="8" t="s">
@@ -1814,7 +1813,7 @@
       <c r="C27" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="27"/>
+      <c r="D27" s="26"/>
       <c r="G27" s="10" t="s">
         <v>13</v>
       </c>
@@ -1826,7 +1825,7 @@
       <c r="C28" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="27"/>
+      <c r="D28" s="26"/>
       <c r="G28" s="10" t="s">
         <v>13</v>
       </c>
@@ -1838,7 +1837,7 @@
       <c r="C29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="27"/>
+      <c r="D29" s="26"/>
       <c r="G29" s="10" t="s">
         <v>13</v>
       </c>
@@ -1850,7 +1849,7 @@
       <c r="C30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="27"/>
+      <c r="D30" s="26"/>
       <c r="G30" s="10" t="s">
         <v>13</v>
       </c>
@@ -1862,7 +1861,7 @@
       <c r="C31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="2:9" ht="13.2">
       <c r="B32" s="8" t="s">
@@ -1871,7 +1870,7 @@
       <c r="C32" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="27"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="2:8" ht="13.2">
       <c r="B33" s="8" t="s">
@@ -1880,20 +1879,20 @@
       <c r="C33" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="27"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D34" s="27"/>
+      <c r="D34" s="26"/>
     </row>
     <row r="35" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D35" s="27"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="2:8" ht="13.2">
       <c r="B36" s="6"/>
       <c r="C36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="27"/>
+      <c r="D36" s="26"/>
     </row>
     <row r="37" spans="2:8" ht="13.2">
       <c r="B37" s="8" t="s">
@@ -1902,7 +1901,7 @@
       <c r="C37" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="28"/>
       <c r="H37" s="10" t="s">
         <v>13</v>
       </c>
@@ -1914,7 +1913,7 @@
       <c r="C38" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="29"/>
+      <c r="D38" s="28"/>
     </row>
     <row r="39" spans="2:8" ht="13.2">
       <c r="B39" s="8" t="s">
@@ -1923,7 +1922,7 @@
       <c r="C39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="29"/>
+      <c r="D39" s="28"/>
       <c r="H39" s="10" t="s">
         <v>13</v>
       </c>
@@ -1935,7 +1934,7 @@
       <c r="C40" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="29"/>
+      <c r="D40" s="28"/>
     </row>
     <row r="41" spans="2:8" ht="13.2">
       <c r="B41" s="8" t="s">
@@ -1944,7 +1943,7 @@
       <c r="C41" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="27"/>
+      <c r="D41" s="26"/>
       <c r="E41" s="10" t="s">
         <v>13</v>
       </c>
@@ -1959,7 +1958,7 @@
       <c r="C42" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="29"/>
+      <c r="D42" s="28"/>
       <c r="E42" s="10" t="s">
         <v>13</v>
       </c>
@@ -1971,7 +1970,7 @@
       <c r="C43" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="27"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="13"/>
       <c r="H43" s="10" t="s">
         <v>13</v>
@@ -1984,7 +1983,7 @@
       <c r="C44" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="27"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="10" t="s">
         <v>13</v>
       </c>
@@ -1996,7 +1995,7 @@
       <c r="C45" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="27"/>
+      <c r="D45" s="26"/>
       <c r="E45" s="13" t="s">
         <v>13</v>
       </c>
@@ -2008,7 +2007,7 @@
       <c r="C46" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="29"/>
+      <c r="D46" s="28"/>
       <c r="E46" s="10" t="s">
         <v>13</v>
       </c>
@@ -2020,7 +2019,7 @@
       <c r="C47" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="29"/>
+      <c r="D47" s="28"/>
       <c r="H47" s="10" t="s">
         <v>13</v>
       </c>
@@ -2032,7 +2031,7 @@
       <c r="C48" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="27"/>
+      <c r="D48" s="26"/>
     </row>
     <row r="49" spans="2:8" ht="13.2">
       <c r="B49" s="8" t="s">
@@ -2041,7 +2040,7 @@
       <c r="C49" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="27"/>
+      <c r="D49" s="26"/>
       <c r="H49" s="10" t="s">
         <v>13</v>
       </c>
@@ -2053,7 +2052,7 @@
       <c r="C50" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D50" s="27"/>
+      <c r="D50" s="26"/>
     </row>
     <row r="51" spans="2:8" ht="13.2">
       <c r="B51" s="8" t="s">
@@ -2062,7 +2061,7 @@
       <c r="C51" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="29"/>
+      <c r="D51" s="28"/>
       <c r="F51" s="11" t="s">
         <v>13</v>
       </c>
@@ -2074,7 +2073,7 @@
       <c r="C52" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="29"/>
+      <c r="D52" s="28"/>
     </row>
     <row r="53" spans="2:8" ht="13.2">
       <c r="B53" s="8" t="s">
@@ -2083,7 +2082,7 @@
       <c r="C53" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="27"/>
+      <c r="D53" s="26"/>
       <c r="H53" s="10" t="s">
         <v>13</v>
       </c>
@@ -2095,7 +2094,7 @@
       <c r="C54" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D54" s="27"/>
+      <c r="D54" s="26"/>
     </row>
     <row r="55" spans="2:8" ht="13.2">
       <c r="B55" s="8" t="s">
@@ -2104,7 +2103,7 @@
       <c r="C55" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D55" s="27"/>
+      <c r="D55" s="26"/>
       <c r="F55" s="10" t="s">
         <v>13</v>
       </c>
@@ -2116,17 +2115,17 @@
       <c r="C56" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D56" s="27"/>
+      <c r="D56" s="26"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D57" s="27"/>
+      <c r="D57" s="26"/>
     </row>
     <row r="58" spans="2:8" ht="13.2">
       <c r="B58" s="6"/>
       <c r="C58" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="27"/>
+      <c r="D58" s="26"/>
     </row>
     <row r="59" spans="2:8" ht="13.2">
       <c r="B59" s="8" t="s">
@@ -2135,7 +2134,7 @@
       <c r="C59" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D59" s="27"/>
+      <c r="D59" s="26"/>
     </row>
     <row r="60" spans="2:8" ht="13.2">
       <c r="B60" s="8" t="s">
@@ -2144,7 +2143,7 @@
       <c r="C60" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D60" s="27"/>
+      <c r="D60" s="26"/>
     </row>
     <row r="61" spans="2:8" ht="13.2">
       <c r="B61" s="8" t="s">
@@ -2153,7 +2152,7 @@
       <c r="C61" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D61" s="27"/>
+      <c r="D61" s="26"/>
       <c r="H61" s="11"/>
     </row>
     <row r="62" spans="2:8" ht="13.2">
@@ -2163,7 +2162,7 @@
       <c r="C62" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="27"/>
+      <c r="D62" s="26"/>
       <c r="H62" s="11" t="s">
         <v>13</v>
       </c>
@@ -2175,13 +2174,13 @@
       <c r="C63" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="27"/>
+      <c r="D63" s="26"/>
       <c r="H63" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="64" spans="2:8" ht="13.2">
-      <c r="D64" s="27"/>
+      <c r="D64" s="26"/>
       <c r="H64" s="11" t="s">
         <v>13</v>
       </c>
@@ -2191,7 +2190,7 @@
       <c r="C65" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D65" s="27"/>
+      <c r="D65" s="26"/>
     </row>
     <row r="66" spans="2:9" ht="13.2">
       <c r="B66" s="8" t="s">
@@ -2200,7 +2199,7 @@
       <c r="C66" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D66" s="27"/>
+      <c r="D66" s="26"/>
     </row>
     <row r="67" spans="2:9" ht="13.2">
       <c r="B67" s="8" t="s">
@@ -2209,7 +2208,7 @@
       <c r="C67" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D67" s="27"/>
+      <c r="D67" s="28"/>
     </row>
     <row r="68" spans="2:9" ht="13.2">
       <c r="B68" s="8" t="s">
@@ -2218,7 +2217,7 @@
       <c r="C68" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="27"/>
+      <c r="D68" s="28"/>
     </row>
     <row r="69" spans="2:9" ht="13.2">
       <c r="B69" s="8" t="s">
@@ -2227,7 +2226,7 @@
       <c r="C69" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D69" s="27"/>
+      <c r="D69" s="28"/>
     </row>
     <row r="70" spans="2:9" ht="13.2">
       <c r="B70" s="8" t="s">
@@ -2236,7 +2235,7 @@
       <c r="C70" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D70" s="27"/>
+      <c r="D70" s="28"/>
       <c r="H70" s="5" t="s">
         <v>13</v>
       </c>
@@ -2248,7 +2247,7 @@
       <c r="C71" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D71" s="27"/>
+      <c r="D71" s="28"/>
     </row>
     <row r="72" spans="2:9" ht="13.2">
       <c r="B72" s="8" t="s">
@@ -2257,7 +2256,7 @@
       <c r="C72" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D72" s="27"/>
+      <c r="D72" s="28"/>
       <c r="E72" s="10" t="s">
         <v>13</v>
       </c>
@@ -2269,7 +2268,7 @@
       <c r="C73" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D73" s="27"/>
+      <c r="D73" s="28"/>
     </row>
     <row r="74" spans="2:9" ht="13.2">
       <c r="B74" s="8" t="s">
@@ -2278,7 +2277,7 @@
       <c r="C74" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D74" s="27"/>
+      <c r="D74" s="28"/>
     </row>
     <row r="75" spans="2:9" ht="13.2">
       <c r="B75" s="8" t="s">
@@ -2287,7 +2286,7 @@
       <c r="C75" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="27"/>
+      <c r="D75" s="26"/>
     </row>
     <row r="76" spans="2:9" ht="13.2">
       <c r="B76" s="8" t="s">
@@ -2296,7 +2295,7 @@
       <c r="C76" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D76" s="27"/>
+      <c r="D76" s="26"/>
       <c r="H76" s="10" t="s">
         <v>13</v>
       </c>
@@ -2308,17 +2307,17 @@
       <c r="C77" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D77" s="27"/>
+      <c r="D77" s="26"/>
     </row>
     <row r="78" spans="2:9" ht="15.75" customHeight="1">
-      <c r="D78" s="27"/>
+      <c r="D78" s="26"/>
     </row>
     <row r="79" spans="2:9" ht="13.2">
       <c r="B79" s="6"/>
       <c r="C79" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D79" s="27"/>
+      <c r="D79" s="26"/>
       <c r="I79" s="10" t="s">
         <v>13</v>
       </c>
@@ -2330,7 +2329,7 @@
       <c r="C80" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="27"/>
+      <c r="D80" s="26"/>
       <c r="G80" s="10" t="s">
         <v>13</v>
       </c>
@@ -2342,7 +2341,7 @@
       <c r="C81" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="27"/>
+      <c r="D81" s="26"/>
     </row>
     <row r="82" spans="2:9" ht="15">
       <c r="B82" s="8" t="s">
@@ -2351,7 +2350,7 @@
       <c r="C82" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D82" s="27"/>
+      <c r="D82" s="26"/>
       <c r="F82" s="10" t="s">
         <v>13</v>
       </c>
@@ -2366,7 +2365,7 @@
       <c r="C83" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D83" s="27"/>
+      <c r="D83" s="26"/>
     </row>
     <row r="84" spans="2:9" ht="15">
       <c r="B84" s="8" t="s">
@@ -2375,7 +2374,7 @@
       <c r="C84" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D84" s="27"/>
+      <c r="D84" s="26"/>
     </row>
     <row r="85" spans="2:9" ht="15">
       <c r="B85" s="8" t="s">
@@ -2384,7 +2383,7 @@
       <c r="C85" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D85" s="27"/>
+      <c r="D85" s="26"/>
       <c r="E85" s="5" t="s">
         <v>13</v>
       </c>
@@ -2396,7 +2395,7 @@
       <c r="C86" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D86" s="27"/>
+      <c r="D86" s="26"/>
     </row>
     <row r="87" spans="2:9" ht="15">
       <c r="B87" s="8" t="s">
@@ -2405,7 +2404,7 @@
       <c r="C87" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D87" s="27"/>
+      <c r="D87" s="26"/>
       <c r="I87" s="11" t="s">
         <v>13</v>
       </c>
@@ -2417,7 +2416,7 @@
       <c r="C88" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D88" s="27"/>
+      <c r="D88" s="26"/>
     </row>
     <row r="89" spans="2:9" ht="13.2">
       <c r="B89" s="8" t="s">
@@ -2426,7 +2425,7 @@
       <c r="C89" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D89" s="27"/>
+      <c r="D89" s="26"/>
       <c r="G89" s="10" t="s">
         <v>13</v>
       </c>
@@ -2438,7 +2437,7 @@
       <c r="C90" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D90" s="27"/>
+      <c r="D90" s="26"/>
     </row>
     <row r="91" spans="2:9" ht="13.2">
       <c r="B91" s="8" t="s">
@@ -2447,7 +2446,7 @@
       <c r="C91" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D91" s="27"/>
+      <c r="D91" s="26"/>
       <c r="I91" s="10" t="s">
         <v>13</v>
       </c>
@@ -2459,7 +2458,7 @@
       <c r="C92" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D92" s="27"/>
+      <c r="D92" s="26"/>
       <c r="H92" s="10" t="s">
         <v>13</v>
       </c>
@@ -2471,7 +2470,7 @@
       <c r="C93" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D93" s="27"/>
+      <c r="D93" s="26"/>
     </row>
     <row r="94" spans="2:9" ht="15">
       <c r="B94" s="8" t="s">
@@ -2480,20 +2479,20 @@
       <c r="C94" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D94" s="27"/>
+      <c r="D94" s="26"/>
       <c r="F94" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="95" spans="2:9" ht="15.75" customHeight="1">
-      <c r="D95" s="27"/>
+      <c r="D95" s="26"/>
     </row>
     <row r="96" spans="2:9" ht="13.2">
       <c r="B96" s="6"/>
       <c r="C96" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D96" s="27"/>
+      <c r="D96" s="26"/>
     </row>
     <row r="97" spans="2:9" ht="13.2">
       <c r="B97" s="8" t="s">
@@ -2502,7 +2501,7 @@
       <c r="C97" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D97" s="27"/>
+      <c r="D97" s="26"/>
     </row>
     <row r="98" spans="2:9" ht="13.2">
       <c r="B98" s="8" t="s">
@@ -2511,7 +2510,7 @@
       <c r="C98" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D98" s="27"/>
+      <c r="D98" s="26"/>
       <c r="E98" s="10" t="s">
         <v>13</v>
       </c>
@@ -2523,7 +2522,7 @@
       <c r="C99" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D99" s="27"/>
+      <c r="D99" s="26"/>
       <c r="I99" s="10" t="s">
         <v>13</v>
       </c>
@@ -2535,7 +2534,7 @@
       <c r="C100" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D100" s="27"/>
+      <c r="D100" s="26"/>
     </row>
     <row r="101" spans="2:9" ht="13.2">
       <c r="B101" s="8" t="s">
@@ -2544,7 +2543,7 @@
       <c r="C101" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D101" s="27"/>
+      <c r="D101" s="26"/>
     </row>
     <row r="102" spans="2:9" ht="13.2">
       <c r="B102" s="8" t="s">
@@ -2553,7 +2552,7 @@
       <c r="C102" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D102" s="27"/>
+      <c r="D102" s="26"/>
       <c r="H102" s="11" t="s">
         <v>13</v>
       </c>
@@ -2565,7 +2564,7 @@
       <c r="C103" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D103" s="27"/>
+      <c r="D103" s="26"/>
       <c r="H103" s="10" t="s">
         <v>13</v>
       </c>
@@ -2580,7 +2579,7 @@
       <c r="C104" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D104" s="27"/>
+      <c r="D104" s="26"/>
       <c r="H104" s="11"/>
     </row>
     <row r="105" spans="2:9" ht="13.2">
@@ -2590,7 +2589,7 @@
       <c r="C105" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D105" s="27"/>
+      <c r="D105" s="26"/>
       <c r="H105" s="10" t="s">
         <v>13</v>
       </c>
@@ -2602,7 +2601,7 @@
       <c r="C106" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D106" s="27"/>
+      <c r="D106" s="26"/>
     </row>
     <row r="107" spans="2:9" ht="13.2">
       <c r="B107" s="8" t="s">
@@ -2611,7 +2610,7 @@
       <c r="C107" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D107" s="27"/>
+      <c r="D107" s="26"/>
       <c r="H107" s="11" t="s">
         <v>13</v>
       </c>
@@ -2626,7 +2625,7 @@
       <c r="C108" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D108" s="27"/>
+      <c r="D108" s="26"/>
     </row>
     <row r="109" spans="2:9" ht="13.2">
       <c r="B109" s="8" t="s">
@@ -2635,7 +2634,7 @@
       <c r="C109" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D109" s="27"/>
+      <c r="D109" s="26"/>
     </row>
     <row r="110" spans="2:9" ht="13.2">
       <c r="B110" s="8" t="s">
@@ -2644,7 +2643,7 @@
       <c r="C110" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D110" s="27"/>
+      <c r="D110" s="26"/>
       <c r="F110" s="11" t="s">
         <v>13</v>
       </c>
@@ -2656,7 +2655,7 @@
       <c r="C111" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D111" s="27"/>
+      <c r="D111" s="26"/>
     </row>
     <row r="112" spans="2:9" ht="13.2">
       <c r="B112" s="8" t="s">
@@ -2665,7 +2664,7 @@
       <c r="C112" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D112" s="27"/>
+      <c r="D112" s="26"/>
     </row>
     <row r="113" spans="2:9" ht="13.2">
       <c r="B113" s="8" t="s">
@@ -2674,7 +2673,7 @@
       <c r="C113" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D113" s="27"/>
+      <c r="D113" s="26"/>
       <c r="I113" s="11" t="s">
         <v>13</v>
       </c>
@@ -2686,7 +2685,7 @@
       <c r="C114" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D114" s="27"/>
+      <c r="D114" s="26"/>
       <c r="H114" s="11" t="s">
         <v>13</v>
       </c>
@@ -2698,7 +2697,7 @@
       <c r="C115" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D115" s="27"/>
+      <c r="D115" s="26"/>
     </row>
     <row r="116" spans="2:9" ht="13.2">
       <c r="B116" s="8" t="s">
@@ -2707,7 +2706,7 @@
       <c r="C116" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D116" s="27"/>
+      <c r="D116" s="26"/>
     </row>
     <row r="117" spans="2:9" ht="13.2">
       <c r="B117" s="8" t="s">
@@ -2716,7 +2715,7 @@
       <c r="C117" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D117" s="27"/>
+      <c r="D117" s="26"/>
     </row>
     <row r="118" spans="2:9" ht="13.2">
       <c r="B118" s="8" t="s">
@@ -2725,7 +2724,7 @@
       <c r="C118" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D118" s="27"/>
+      <c r="D118" s="26"/>
     </row>
     <row r="119" spans="2:9" ht="13.2">
       <c r="B119" s="8" t="s">
@@ -2734,7 +2733,7 @@
       <c r="C119" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D119" s="27"/>
+      <c r="D119" s="26"/>
       <c r="F119" s="11" t="s">
         <v>13</v>
       </c>
@@ -2746,7 +2745,7 @@
       <c r="C120" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D120" s="27"/>
+      <c r="D120" s="26"/>
       <c r="I120" s="11" t="s">
         <v>13</v>
       </c>
@@ -2758,7 +2757,7 @@
       <c r="C121" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D121" s="27"/>
+      <c r="D121" s="26"/>
     </row>
     <row r="122" spans="2:9" ht="13.2">
       <c r="B122" s="8" t="s">
@@ -2767,16 +2766,16 @@
       <c r="C122" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D122" s="27"/>
+      <c r="D122" s="26"/>
     </row>
     <row r="123" spans="2:9" ht="15.75" customHeight="1">
-      <c r="D123" s="27"/>
+      <c r="D123" s="26"/>
     </row>
     <row r="124" spans="2:9" ht="13.2">
-      <c r="C124" s="20" t="s">
+      <c r="C124" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D124" s="27"/>
+      <c r="D124" s="26"/>
     </row>
     <row r="125" spans="2:9" ht="13.2">
       <c r="B125" s="8" t="s">
@@ -2785,7 +2784,7 @@
       <c r="C125" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D125" s="27"/>
+      <c r="D125" s="26"/>
     </row>
     <row r="126" spans="2:9" ht="13.2">
       <c r="B126" s="8" t="s">
@@ -2794,7 +2793,7 @@
       <c r="C126" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D126" s="27"/>
+      <c r="D126" s="26"/>
       <c r="E126" s="11" t="s">
         <v>13</v>
       </c>
@@ -2806,7 +2805,7 @@
       <c r="C127" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D127" s="27"/>
+      <c r="D127" s="26"/>
       <c r="G127" s="11" t="s">
         <v>13</v>
       </c>
@@ -2821,7 +2820,7 @@
       <c r="C128" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D128" s="27"/>
+      <c r="D128" s="26"/>
     </row>
     <row r="129" spans="2:9" ht="13.2">
       <c r="B129" s="8" t="s">
@@ -2830,7 +2829,7 @@
       <c r="C129" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D129" s="27"/>
+      <c r="D129" s="26"/>
       <c r="H129" s="11" t="s">
         <v>13</v>
       </c>
@@ -2839,10 +2838,10 @@
       <c r="B130" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C130" s="21" t="s">
+      <c r="C130" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="D130" s="27"/>
+      <c r="D130" s="26"/>
     </row>
     <row r="131" spans="2:9" ht="13.2">
       <c r="B131" s="8" t="s">
@@ -2851,7 +2850,7 @@
       <c r="C131" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D131" s="27"/>
+      <c r="D131" s="26"/>
     </row>
     <row r="132" spans="2:9" ht="13.2">
       <c r="B132" s="8" t="s">
@@ -2860,7 +2859,7 @@
       <c r="C132" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D132" s="27"/>
+      <c r="D132" s="26"/>
       <c r="I132" s="11" t="s">
         <v>13</v>
       </c>
@@ -2872,7 +2871,7 @@
       <c r="C133" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D133" s="27"/>
+      <c r="D133" s="26"/>
       <c r="E133" s="11" t="s">
         <v>13</v>
       </c>
@@ -2884,7 +2883,7 @@
       <c r="C134" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D134" s="27"/>
+      <c r="D134" s="26"/>
       <c r="G134" s="11" t="s">
         <v>13</v>
       </c>
@@ -2896,7 +2895,7 @@
       <c r="C135" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D135" s="27"/>
+      <c r="D135" s="26"/>
       <c r="H135" s="11" t="s">
         <v>13</v>
       </c>
@@ -2908,7 +2907,7 @@
       <c r="C136" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D136" s="27"/>
+      <c r="D136" s="26"/>
     </row>
     <row r="137" spans="2:9" ht="13.2">
       <c r="B137" s="8" t="s">
@@ -2917,7 +2916,7 @@
       <c r="C137" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D137" s="27"/>
+      <c r="D137" s="26"/>
       <c r="E137" s="11" t="s">
         <v>13</v>
       </c>
@@ -2929,7 +2928,7 @@
       <c r="C138" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D138" s="27"/>
+      <c r="D138" s="26"/>
     </row>
     <row r="139" spans="2:9" ht="13.2">
       <c r="B139" s="8" t="s">
@@ -2938,7 +2937,7 @@
       <c r="C139" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D139" s="27"/>
+      <c r="D139" s="26"/>
       <c r="G139" s="11" t="s">
         <v>13</v>
       </c>
@@ -2953,7 +2952,7 @@
       <c r="C140" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D140" s="27"/>
+      <c r="D140" s="26"/>
       <c r="I140" s="11" t="s">
         <v>13</v>
       </c>
@@ -2962,23 +2961,23 @@
       <c r="B141" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C141" s="22" t="s">
+      <c r="C141" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="D141" s="27"/>
+      <c r="D141" s="26"/>
     </row>
     <row r="142" spans="2:9" ht="13.2">
-      <c r="D142" s="27"/>
+      <c r="D142" s="26"/>
       <c r="G142" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="143" spans="2:9" ht="13.2">
       <c r="B143" s="6"/>
-      <c r="C143" s="23" t="s">
+      <c r="C143" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="D143" s="27"/>
+      <c r="D143" s="26"/>
     </row>
     <row r="144" spans="2:9" ht="13.2">
       <c r="B144" s="8" t="s">
@@ -2987,7 +2986,7 @@
       <c r="C144" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D144" s="27"/>
+      <c r="D144" s="26"/>
     </row>
     <row r="145" spans="2:9" ht="13.2">
       <c r="B145" s="8" t="s">
@@ -2996,7 +2995,7 @@
       <c r="C145" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D145" s="27"/>
+      <c r="D145" s="26"/>
       <c r="F145" s="11" t="s">
         <v>13</v>
       </c>
@@ -3008,7 +3007,7 @@
       <c r="C146" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D146" s="27"/>
+      <c r="D146" s="26"/>
       <c r="F146" s="11" t="s">
         <v>13</v>
       </c>
@@ -3023,7 +3022,7 @@
       <c r="C147" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D147" s="27"/>
+      <c r="D147" s="26"/>
       <c r="F147" s="11"/>
     </row>
     <row r="148" spans="2:9" ht="13.2">
@@ -3033,7 +3032,7 @@
       <c r="C148" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D148" s="28" t="s">
+      <c r="D148" s="27" t="s">
         <v>13</v>
       </c>
       <c r="F148" s="11" t="s">
@@ -3047,7 +3046,7 @@
       <c r="C149" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D149" s="27"/>
+      <c r="D149" s="26"/>
     </row>
     <row r="150" spans="2:9" ht="13.2">
       <c r="B150" s="8" t="s">
@@ -3056,7 +3055,7 @@
       <c r="C150" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D150" s="27"/>
+      <c r="D150" s="26"/>
     </row>
     <row r="151" spans="2:9" ht="13.2">
       <c r="B151" s="8" t="s">
@@ -3065,7 +3064,7 @@
       <c r="C151" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D151" s="27"/>
+      <c r="D151" s="26"/>
     </row>
     <row r="152" spans="2:9" ht="13.2">
       <c r="B152" s="8" t="s">
@@ -3074,7 +3073,7 @@
       <c r="C152" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D152" s="27"/>
+      <c r="D152" s="26"/>
       <c r="G152" s="5" t="s">
         <v>13</v>
       </c>
@@ -3089,7 +3088,7 @@
       <c r="C153" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D153" s="27"/>
+      <c r="D153" s="26"/>
     </row>
     <row r="154" spans="2:9" ht="13.2">
       <c r="B154" s="8" t="s">
@@ -3098,7 +3097,7 @@
       <c r="C154" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D154" s="28" t="s">
+      <c r="D154" s="27" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3109,7 +3108,7 @@
       <c r="C155" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D155" s="27"/>
+      <c r="D155" s="26"/>
     </row>
     <row r="156" spans="2:9" ht="13.2">
       <c r="B156" s="8" t="s">
@@ -3118,7 +3117,7 @@
       <c r="C156" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D156" s="27"/>
+      <c r="D156" s="26"/>
     </row>
     <row r="157" spans="2:9" ht="13.2">
       <c r="B157" s="8" t="s">
@@ -3127,7 +3126,7 @@
       <c r="C157" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D157" s="27"/>
+      <c r="D157" s="26"/>
       <c r="G157" s="11" t="s">
         <v>13</v>
       </c>
@@ -3142,7 +3141,7 @@
       <c r="C158" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D158" s="27"/>
+      <c r="D158" s="26"/>
       <c r="I158" s="11" t="s">
         <v>13</v>
       </c>
@@ -3154,7 +3153,7 @@
       <c r="C159" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D159" s="27"/>
+      <c r="D159" s="26"/>
     </row>
     <row r="160" spans="2:9" ht="13.2">
       <c r="B160" s="8" t="s">
@@ -3163,7 +3162,7 @@
       <c r="C160" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D160" s="27"/>
+      <c r="D160" s="26"/>
     </row>
     <row r="161" spans="2:9" ht="13.2">
       <c r="B161" s="8" t="s">
@@ -3172,7 +3171,7 @@
       <c r="C161" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D161" s="27"/>
+      <c r="D161" s="26"/>
     </row>
     <row r="162" spans="2:9" ht="13.2">
       <c r="B162" s="8" t="s">
@@ -3181,7 +3180,7 @@
       <c r="C162" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D162" s="27"/>
+      <c r="D162" s="26"/>
     </row>
     <row r="163" spans="2:9" ht="13.2">
       <c r="B163" s="8" t="s">
@@ -3190,7 +3189,7 @@
       <c r="C163" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D163" s="27"/>
+      <c r="D163" s="26"/>
     </row>
     <row r="164" spans="2:9" ht="13.2">
       <c r="B164" s="8" t="s">
@@ -3199,7 +3198,7 @@
       <c r="C164" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D164" s="27"/>
+      <c r="D164" s="26"/>
     </row>
     <row r="165" spans="2:9" ht="13.2">
       <c r="B165" s="8" t="s">
@@ -3208,7 +3207,7 @@
       <c r="C165" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D165" s="27"/>
+      <c r="D165" s="26"/>
       <c r="I165" s="5" t="s">
         <v>13</v>
       </c>
@@ -3220,7 +3219,7 @@
       <c r="C166" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D166" s="27"/>
+      <c r="D166" s="26"/>
       <c r="E166" s="11" t="s">
         <v>13</v>
       </c>
@@ -3232,7 +3231,7 @@
       <c r="C167" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D167" s="27"/>
+      <c r="D167" s="26"/>
     </row>
     <row r="168" spans="2:9" ht="13.2">
       <c r="B168" s="8" t="s">
@@ -3241,7 +3240,7 @@
       <c r="C168" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D168" s="27"/>
+      <c r="D168" s="26"/>
     </row>
     <row r="169" spans="2:9" ht="13.2">
       <c r="B169" s="8" t="s">
@@ -3250,7 +3249,7 @@
       <c r="C169" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D169" s="27"/>
+      <c r="D169" s="26"/>
     </row>
     <row r="170" spans="2:9" ht="13.2">
       <c r="B170" s="8" t="s">
@@ -3259,7 +3258,7 @@
       <c r="C170" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D170" s="27"/>
+      <c r="D170" s="26"/>
       <c r="I170" s="11" t="s">
         <v>13</v>
       </c>
@@ -3271,7 +3270,7 @@
       <c r="C171" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D171" s="27"/>
+      <c r="D171" s="26"/>
       <c r="F171" s="11" t="s">
         <v>13</v>
       </c>
@@ -3286,7 +3285,7 @@
       <c r="C172" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D172" s="27"/>
+      <c r="D172" s="26"/>
       <c r="E172" s="11" t="s">
         <v>13</v>
       </c>
@@ -3304,7 +3303,7 @@
       <c r="C173" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D173" s="27"/>
+      <c r="D173" s="26"/>
       <c r="H173" s="11" t="s">
         <v>13</v>
       </c>
@@ -3316,7 +3315,7 @@
       <c r="C174" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D174" s="27"/>
+      <c r="D174" s="26"/>
       <c r="G174" s="11" t="s">
         <v>13</v>
       </c>
@@ -3334,7 +3333,7 @@
       <c r="C175" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D175" s="27"/>
+      <c r="D175" s="26"/>
     </row>
     <row r="176" spans="2:9" ht="13.2">
       <c r="B176" s="8" t="s">
@@ -3343,7 +3342,7 @@
       <c r="C176" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D176" s="27"/>
+      <c r="D176" s="26"/>
     </row>
     <row r="177" spans="2:9" ht="13.2">
       <c r="B177" s="8" t="s">
@@ -3352,7 +3351,7 @@
       <c r="C177" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="D177" s="27"/>
+      <c r="D177" s="26"/>
       <c r="F177" s="11" t="s">
         <v>13</v>
       </c>
@@ -3364,7 +3363,7 @@
       <c r="C178" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D178" s="27"/>
+      <c r="D178" s="26"/>
       <c r="E178" s="11" t="s">
         <v>13</v>
       </c>
@@ -3376,7 +3375,7 @@
       <c r="C179" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D179" s="27"/>
+      <c r="D179" s="26"/>
       <c r="H179" s="11" t="s">
         <v>13</v>
       </c>
@@ -3388,16 +3387,16 @@
       <c r="C180" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="D180" s="27"/>
+      <c r="D180" s="26"/>
     </row>
     <row r="181" spans="2:9" ht="13.2">
       <c r="B181" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C181" s="21" t="s">
+      <c r="C181" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D181" s="27"/>
+      <c r="D181" s="26"/>
       <c r="F181" s="11" t="s">
         <v>13</v>
       </c>
@@ -3412,7 +3411,7 @@
       <c r="C182" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D182" s="27"/>
+      <c r="D182" s="26"/>
     </row>
     <row r="183" spans="2:9" ht="13.2">
       <c r="B183" s="8" t="s">
@@ -3421,7 +3420,7 @@
       <c r="C183" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D183" s="27"/>
+      <c r="D183" s="26"/>
       <c r="G183" s="11" t="s">
         <v>13</v>
       </c>
@@ -3433,7 +3432,7 @@
       <c r="C184" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D184" s="27"/>
+      <c r="D184" s="26"/>
       <c r="H184" s="11" t="s">
         <v>13</v>
       </c>
@@ -3445,7 +3444,7 @@
       <c r="C185" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D185" s="27"/>
+      <c r="D185" s="26"/>
       <c r="F185" s="11" t="s">
         <v>13</v>
       </c>
@@ -3460,7 +3459,7 @@
       <c r="C186" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D186" s="27"/>
+      <c r="D186" s="26"/>
       <c r="F186" s="11" t="s">
         <v>13</v>
       </c>
@@ -3472,7 +3471,7 @@
       <c r="C187" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D187" s="27"/>
+      <c r="D187" s="26"/>
       <c r="F187" s="11" t="s">
         <v>13</v>
       </c>
@@ -3484,7 +3483,7 @@
       <c r="C188" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D188" s="27"/>
+      <c r="D188" s="26"/>
       <c r="F188" s="11" t="s">
         <v>13</v>
       </c>
@@ -3496,7 +3495,7 @@
       <c r="C189" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="D189" s="27"/>
+      <c r="D189" s="26"/>
     </row>
     <row r="190" spans="2:9" ht="13.2">
       <c r="B190" s="8" t="s">
@@ -3505,7 +3504,7 @@
       <c r="C190" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D190" s="27"/>
+      <c r="D190" s="26"/>
       <c r="I190" s="11" t="s">
         <v>13</v>
       </c>
@@ -3517,17 +3516,17 @@
       <c r="C191" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D191" s="27"/>
+      <c r="D191" s="26"/>
     </row>
     <row r="192" spans="2:9" ht="15.75" customHeight="1">
-      <c r="D192" s="27"/>
+      <c r="D192" s="26"/>
     </row>
     <row r="193" spans="2:7" ht="13.2">
       <c r="B193" s="6"/>
       <c r="C193" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D193" s="27"/>
+      <c r="D193" s="26"/>
     </row>
     <row r="194" spans="2:7" ht="13.2">
       <c r="B194" s="8" t="s">
@@ -3536,7 +3535,7 @@
       <c r="C194" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D194" s="27"/>
+      <c r="D194" s="26"/>
       <c r="G194" s="11" t="s">
         <v>13</v>
       </c>
@@ -3548,7 +3547,7 @@
       <c r="C195" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D195" s="27"/>
+      <c r="D195" s="26"/>
       <c r="E195" s="11" t="s">
         <v>13</v>
       </c>
@@ -3560,7 +3559,7 @@
       <c r="C196" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="D196" s="27"/>
+      <c r="D196" s="26"/>
     </row>
     <row r="197" spans="2:7" ht="13.2">
       <c r="B197" s="8" t="s">
@@ -3569,7 +3568,7 @@
       <c r="C197" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D197" s="27"/>
+      <c r="D197" s="26"/>
       <c r="G197" s="11" t="s">
         <v>13</v>
       </c>
@@ -3581,7 +3580,7 @@
       <c r="C198" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="D198" s="27"/>
+      <c r="D198" s="26"/>
     </row>
     <row r="199" spans="2:7" ht="13.2">
       <c r="B199" s="8" t="s">
@@ -3590,7 +3589,7 @@
       <c r="C199" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="D199" s="27"/>
+      <c r="D199" s="26"/>
     </row>
     <row r="200" spans="2:7" ht="13.2">
       <c r="B200" s="8" t="s">
@@ -3599,7 +3598,7 @@
       <c r="C200" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D200" s="27"/>
+      <c r="D200" s="26"/>
     </row>
     <row r="201" spans="2:7" ht="13.2">
       <c r="B201" s="8" t="s">
@@ -3608,7 +3607,7 @@
       <c r="C201" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D201" s="27"/>
+      <c r="D201" s="26"/>
       <c r="E201" s="11" t="s">
         <v>13</v>
       </c>
@@ -3620,7 +3619,7 @@
       <c r="C202" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="D202" s="27"/>
+      <c r="D202" s="26"/>
       <c r="E202" s="11" t="s">
         <v>13</v>
       </c>
@@ -3632,7 +3631,7 @@
       <c r="C203" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D203" s="27"/>
+      <c r="D203" s="26"/>
       <c r="E203" s="11" t="s">
         <v>13</v>
       </c>
@@ -3644,7 +3643,7 @@
       <c r="C204" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="D204" s="27"/>
+      <c r="D204" s="26"/>
       <c r="E204" s="11" t="s">
         <v>13</v>
       </c>
@@ -3659,7 +3658,7 @@
       <c r="C205" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D205" s="27"/>
+      <c r="D205" s="26"/>
     </row>
     <row r="206" spans="2:7" ht="13.2">
       <c r="B206" s="8" t="s">
@@ -3668,7 +3667,7 @@
       <c r="C206" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="D206" s="27"/>
+      <c r="D206" s="26"/>
     </row>
     <row r="207" spans="2:7" ht="13.2">
       <c r="B207" s="8" t="s">
@@ -3677,7 +3676,7 @@
       <c r="C207" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D207" s="27"/>
+      <c r="D207" s="26"/>
       <c r="E207" s="11" t="s">
         <v>13</v>
       </c>
@@ -3689,7 +3688,7 @@
       <c r="C208" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="D208" s="27"/>
+      <c r="D208" s="26"/>
     </row>
     <row r="209" spans="2:9" ht="13.2">
       <c r="B209" s="8" t="s">
@@ -3698,7 +3697,7 @@
       <c r="C209" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D209" s="27"/>
+      <c r="D209" s="26"/>
     </row>
     <row r="210" spans="2:9" ht="13.2">
       <c r="B210" s="8" t="s">
@@ -3707,7 +3706,7 @@
       <c r="C210" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="D210" s="27"/>
+      <c r="D210" s="26"/>
     </row>
     <row r="211" spans="2:9" ht="13.2">
       <c r="B211" s="8" t="s">
@@ -3716,7 +3715,7 @@
       <c r="C211" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="D211" s="27"/>
+      <c r="D211" s="26"/>
     </row>
     <row r="212" spans="2:9" ht="13.2">
       <c r="B212" s="8" t="s">
@@ -3725,7 +3724,7 @@
       <c r="C212" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="D212" s="27"/>
+      <c r="D212" s="26"/>
     </row>
     <row r="213" spans="2:9" ht="13.2">
       <c r="B213" s="8" t="s">
@@ -3734,7 +3733,7 @@
       <c r="C213" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="D213" s="27"/>
+      <c r="D213" s="26"/>
       <c r="G213" s="11" t="s">
         <v>13</v>
       </c>
@@ -3746,7 +3745,7 @@
       <c r="C214" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D214" s="27"/>
+      <c r="D214" s="26"/>
     </row>
     <row r="215" spans="2:9" ht="13.2">
       <c r="B215" s="8" t="s">
@@ -3755,7 +3754,7 @@
       <c r="C215" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D215" s="27"/>
+      <c r="D215" s="26"/>
     </row>
     <row r="216" spans="2:9" ht="13.2">
       <c r="B216" s="8" t="s">
@@ -3764,7 +3763,7 @@
       <c r="C216" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D216" s="27"/>
+      <c r="D216" s="26"/>
     </row>
     <row r="217" spans="2:9" ht="13.2">
       <c r="B217" s="8" t="s">
@@ -3773,7 +3772,7 @@
       <c r="C217" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="D217" s="27"/>
+      <c r="D217" s="26"/>
       <c r="I217" s="11" t="s">
         <v>13</v>
       </c>
@@ -3785,7 +3784,7 @@
       <c r="C218" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="D218" s="27"/>
+      <c r="D218" s="26"/>
       <c r="F218" s="11" t="s">
         <v>13</v>
       </c>
@@ -3800,7 +3799,7 @@
       <c r="C219" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="D219" s="27"/>
+      <c r="D219" s="26"/>
     </row>
     <row r="220" spans="2:9" ht="13.2">
       <c r="B220" s="8" t="s">
@@ -3809,7 +3808,7 @@
       <c r="C220" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="D220" s="27"/>
+      <c r="D220" s="26"/>
     </row>
     <row r="221" spans="2:9" ht="13.2">
       <c r="B221" s="8" t="s">
@@ -3818,7 +3817,7 @@
       <c r="C221" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="D221" s="27"/>
+      <c r="D221" s="26"/>
       <c r="E221" s="11" t="s">
         <v>13</v>
       </c>
@@ -3830,7 +3829,7 @@
       <c r="C222" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D222" s="27"/>
+      <c r="D222" s="26"/>
     </row>
     <row r="223" spans="2:9" ht="13.2">
       <c r="B223" s="8" t="s">
@@ -3839,7 +3838,7 @@
       <c r="C223" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="D223" s="27"/>
+      <c r="D223" s="26"/>
       <c r="H223" s="11" t="s">
         <v>13</v>
       </c>
@@ -3854,7 +3853,7 @@
       <c r="C224" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="D224" s="27"/>
+      <c r="D224" s="26"/>
       <c r="G224" s="11" t="s">
         <v>13</v>
       </c>
@@ -3866,7 +3865,7 @@
       <c r="C225" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="D225" s="27"/>
+      <c r="D225" s="26"/>
       <c r="G225" s="11" t="s">
         <v>13</v>
       </c>
@@ -3881,7 +3880,7 @@
       <c r="C226" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D226" s="27"/>
+      <c r="D226" s="26"/>
       <c r="G226" s="11"/>
     </row>
     <row r="227" spans="2:9" ht="13.2">
@@ -3891,7 +3890,7 @@
       <c r="C227" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="D227" s="27"/>
+      <c r="D227" s="26"/>
       <c r="G227" s="11" t="s">
         <v>13</v>
       </c>
@@ -3909,7 +3908,7 @@
       <c r="C228" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="D228" s="27"/>
+      <c r="D228" s="26"/>
     </row>
     <row r="229" spans="2:9" ht="13.2">
       <c r="B229" s="8" t="s">
@@ -3918,7 +3917,7 @@
       <c r="C229" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="D229" s="27"/>
+      <c r="D229" s="26"/>
     </row>
     <row r="230" spans="2:9" ht="13.2">
       <c r="B230" s="8" t="s">
@@ -3927,19 +3926,19 @@
       <c r="C230" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="D230" s="27"/>
+      <c r="D230" s="26"/>
     </row>
     <row r="231" spans="2:9" ht="13.2">
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
-      <c r="D231" s="27"/>
+      <c r="D231" s="26"/>
     </row>
     <row r="232" spans="2:9" ht="13.2">
       <c r="B232" s="6"/>
-      <c r="C232" s="24" t="s">
+      <c r="C232" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="D232" s="27"/>
+      <c r="D232" s="26"/>
     </row>
     <row r="233" spans="2:9" ht="13.2">
       <c r="B233" s="8" t="s">
@@ -3948,7 +3947,7 @@
       <c r="C233" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D233" s="27"/>
+      <c r="D233" s="26"/>
     </row>
     <row r="234" spans="2:9" ht="13.2">
       <c r="B234" s="8" t="s">
@@ -3957,7 +3956,7 @@
       <c r="C234" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="D234" s="27"/>
+      <c r="D234" s="26"/>
       <c r="E234" s="11" t="s">
         <v>13</v>
       </c>
@@ -3969,7 +3968,7 @@
       <c r="C235" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D235" s="27"/>
+      <c r="D235" s="26"/>
       <c r="E235" s="11" t="s">
         <v>13</v>
       </c>
@@ -3981,7 +3980,7 @@
       <c r="C236" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="D236" s="27"/>
+      <c r="D236" s="26"/>
       <c r="E236" s="11" t="s">
         <v>13</v>
       </c>
@@ -3993,7 +3992,7 @@
       <c r="C237" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="D237" s="27"/>
+      <c r="D237" s="26"/>
       <c r="E237" s="11" t="s">
         <v>13</v>
       </c>
@@ -4005,24 +4004,24 @@
       <c r="C238" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="D238" s="27"/>
+      <c r="D238" s="26"/>
     </row>
     <row r="239" spans="2:9" ht="13.2">
       <c r="B239" s="6"/>
       <c r="C239" s="6"/>
-      <c r="D239" s="27"/>
+      <c r="D239" s="26"/>
     </row>
     <row r="240" spans="2:9" ht="13.2">
       <c r="B240" s="6"/>
-      <c r="C240" s="20" t="s">
+      <c r="C240" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="D240" s="27"/>
+      <c r="D240" s="26"/>
     </row>
     <row r="241" spans="2:7" ht="13.2">
       <c r="B241" s="6"/>
       <c r="C241" s="6"/>
-      <c r="D241" s="27"/>
+      <c r="D241" s="26"/>
     </row>
     <row r="242" spans="2:7" ht="13.2">
       <c r="B242" s="8" t="s">
@@ -4031,7 +4030,7 @@
       <c r="C242" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="D242" s="27"/>
+      <c r="D242" s="26"/>
     </row>
     <row r="243" spans="2:7" ht="13.2">
       <c r="B243" s="8" t="s">
@@ -4040,7 +4039,7 @@
       <c r="C243" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D243" s="27"/>
+      <c r="D243" s="26"/>
     </row>
     <row r="244" spans="2:7" ht="13.2">
       <c r="B244" s="8" t="s">
@@ -4049,7 +4048,7 @@
       <c r="C244" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D244" s="27"/>
+      <c r="D244" s="26"/>
     </row>
     <row r="245" spans="2:7" ht="13.2">
       <c r="B245" s="8" t="s">
@@ -4058,7 +4057,7 @@
       <c r="C245" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D245" s="27"/>
+      <c r="D245" s="26"/>
     </row>
     <row r="246" spans="2:7" ht="13.2">
       <c r="B246" s="8" t="s">
@@ -4067,7 +4066,7 @@
       <c r="C246" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D246" s="27"/>
+      <c r="D246" s="26"/>
     </row>
     <row r="247" spans="2:7" ht="13.2">
       <c r="B247" s="8" t="s">
@@ -4076,7 +4075,7 @@
       <c r="C247" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D247" s="27"/>
+      <c r="D247" s="26"/>
     </row>
     <row r="248" spans="2:7" ht="13.2">
       <c r="B248" s="8" t="s">
@@ -4085,7 +4084,7 @@
       <c r="C248" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D248" s="27"/>
+      <c r="D248" s="26"/>
     </row>
     <row r="249" spans="2:7" ht="13.2">
       <c r="B249" s="8" t="s">
@@ -4094,7 +4093,7 @@
       <c r="C249" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="D249" s="27"/>
+      <c r="D249" s="26"/>
     </row>
     <row r="250" spans="2:7" ht="13.2">
       <c r="B250" s="8" t="s">
@@ -4103,7 +4102,7 @@
       <c r="C250" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="D250" s="27"/>
+      <c r="D250" s="26"/>
       <c r="G250" s="11" t="s">
         <v>13</v>
       </c>
@@ -4115,7 +4114,7 @@
       <c r="C251" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D251" s="27"/>
+      <c r="D251" s="26"/>
     </row>
     <row r="252" spans="2:7" ht="13.2">
       <c r="B252" s="8" t="s">
@@ -4124,7 +4123,7 @@
       <c r="C252" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="D252" s="27"/>
+      <c r="D252" s="26"/>
     </row>
     <row r="253" spans="2:7" ht="13.2">
       <c r="B253" s="8" t="s">
@@ -4133,7 +4132,7 @@
       <c r="C253" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="D253" s="27"/>
+      <c r="D253" s="26"/>
       <c r="E253" s="11" t="s">
         <v>13</v>
       </c>
@@ -4145,7 +4144,7 @@
       <c r="C254" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D254" s="27"/>
+      <c r="D254" s="26"/>
     </row>
     <row r="255" spans="2:7" ht="13.2">
       <c r="B255" s="8" t="s">
@@ -4154,19 +4153,19 @@
       <c r="C255" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="D255" s="27"/>
+      <c r="D255" s="26"/>
     </row>
     <row r="256" spans="2:7" ht="13.2">
       <c r="B256" s="6"/>
       <c r="C256" s="6"/>
-      <c r="D256" s="27"/>
+      <c r="D256" s="26"/>
     </row>
     <row r="257" spans="2:9" ht="13.2">
       <c r="B257" s="6"/>
-      <c r="C257" s="24" t="s">
+      <c r="C257" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="D257" s="27"/>
+      <c r="D257" s="26"/>
     </row>
     <row r="258" spans="2:9" ht="13.2">
       <c r="B258" s="8" t="s">
@@ -4175,7 +4174,7 @@
       <c r="C258" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="D258" s="27"/>
+      <c r="D258" s="26"/>
     </row>
     <row r="259" spans="2:9" ht="13.2">
       <c r="B259" s="8" t="s">
@@ -4184,7 +4183,7 @@
       <c r="C259" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="D259" s="27"/>
+      <c r="D259" s="26"/>
       <c r="F259" s="11" t="s">
         <v>13</v>
       </c>
@@ -4196,7 +4195,7 @@
       <c r="C260" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D260" s="27"/>
+      <c r="D260" s="26"/>
       <c r="I260" s="11" t="s">
         <v>13</v>
       </c>
@@ -4208,7 +4207,7 @@
       <c r="C261" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="D261" s="27"/>
+      <c r="D261" s="26"/>
       <c r="H261" s="11" t="s">
         <v>13</v>
       </c>
@@ -4220,7 +4219,7 @@
       <c r="C262" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D262" s="27"/>
+      <c r="D262" s="26"/>
     </row>
     <row r="263" spans="2:9" ht="13.2">
       <c r="B263" s="8" t="s">
@@ -4229,7 +4228,7 @@
       <c r="C263" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="D263" s="27"/>
+      <c r="D263" s="26"/>
     </row>
     <row r="264" spans="2:9" ht="13.2">
       <c r="B264" s="8" t="s">
@@ -4238,7 +4237,7 @@
       <c r="C264" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D264" s="27"/>
+      <c r="D264" s="26"/>
       <c r="E264" s="11" t="s">
         <v>13</v>
       </c>
@@ -4250,7 +4249,7 @@
       <c r="C265" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D265" s="27"/>
+      <c r="D265" s="26"/>
       <c r="E265" s="11" t="s">
         <v>13</v>
       </c>
@@ -4262,7 +4261,7 @@
       <c r="C266" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="D266" s="27"/>
+      <c r="D266" s="26"/>
       <c r="E266" s="11"/>
       <c r="I266" s="11" t="s">
         <v>13</v>
@@ -4275,7 +4274,7 @@
       <c r="C267" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="D267" s="27"/>
+      <c r="D267" s="26"/>
       <c r="E267" s="11" t="s">
         <v>13</v>
       </c>
@@ -4290,7 +4289,7 @@
       <c r="C268" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="D268" s="27"/>
+      <c r="D268" s="26"/>
       <c r="H268" s="11" t="s">
         <v>13</v>
       </c>
@@ -4302,7 +4301,7 @@
       <c r="C269" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="D269" s="27"/>
+      <c r="D269" s="26"/>
       <c r="H269" s="11"/>
     </row>
     <row r="270" spans="2:9" ht="13.2">
@@ -4312,7 +4311,7 @@
       <c r="C270" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="D270" s="27"/>
+      <c r="D270" s="26"/>
       <c r="H270" s="11" t="s">
         <v>13</v>
       </c>
@@ -4324,7 +4323,7 @@
       <c r="C271" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D271" s="27"/>
+      <c r="D271" s="26"/>
       <c r="F271" s="11" t="s">
         <v>13</v>
       </c>
@@ -4336,7 +4335,7 @@
       <c r="C272" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D272" s="27"/>
+      <c r="D272" s="26"/>
     </row>
     <row r="273" spans="2:9" ht="13.2">
       <c r="B273" s="8" t="s">
@@ -4345,7 +4344,7 @@
       <c r="C273" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="D273" s="27"/>
+      <c r="D273" s="26"/>
     </row>
     <row r="274" spans="2:9" ht="13.2">
       <c r="B274" s="8" t="s">
@@ -4354,7 +4353,7 @@
       <c r="C274" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="D274" s="27"/>
+      <c r="D274" s="26"/>
     </row>
     <row r="275" spans="2:9" ht="13.2">
       <c r="B275" s="8" t="s">
@@ -4363,7 +4362,7 @@
       <c r="C275" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="D275" s="27"/>
+      <c r="D275" s="26"/>
     </row>
     <row r="276" spans="2:9" ht="13.2">
       <c r="B276" s="8" t="s">
@@ -4372,7 +4371,7 @@
       <c r="C276" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D276" s="27"/>
+      <c r="D276" s="26"/>
       <c r="H276" s="11" t="s">
         <v>13</v>
       </c>
@@ -4384,7 +4383,7 @@
       <c r="C277" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="D277" s="27"/>
+      <c r="D277" s="26"/>
     </row>
     <row r="278" spans="2:9" ht="13.2">
       <c r="B278" s="8" t="s">
@@ -4393,7 +4392,7 @@
       <c r="C278" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="D278" s="27"/>
+      <c r="D278" s="26"/>
     </row>
     <row r="279" spans="2:9" ht="13.2">
       <c r="B279" s="8" t="s">
@@ -4402,7 +4401,7 @@
       <c r="C279" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D279" s="27"/>
+      <c r="D279" s="26"/>
       <c r="F279" s="11" t="s">
         <v>13</v>
       </c>
@@ -4414,7 +4413,7 @@
       <c r="C280" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D280" s="27"/>
+      <c r="D280" s="26"/>
     </row>
     <row r="281" spans="2:9" ht="13.2">
       <c r="B281" s="8" t="s">
@@ -4423,7 +4422,7 @@
       <c r="C281" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="D281" s="27"/>
+      <c r="D281" s="26"/>
       <c r="I281" s="11" t="s">
         <v>13</v>
       </c>
@@ -4435,7 +4434,7 @@
       <c r="C282" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="D282" s="27"/>
+      <c r="D282" s="26"/>
       <c r="E282" s="11" t="s">
         <v>13</v>
       </c>
@@ -4447,7 +4446,7 @@
       <c r="C283" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="D283" s="27"/>
+      <c r="D283" s="26"/>
       <c r="E283" s="11" t="s">
         <v>13</v>
       </c>
@@ -4459,7 +4458,7 @@
       <c r="C284" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D284" s="27"/>
+      <c r="D284" s="26"/>
       <c r="E284" s="11" t="s">
         <v>13</v>
       </c>
@@ -4471,7 +4470,7 @@
       <c r="C285" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="D285" s="27"/>
+      <c r="D285" s="26"/>
       <c r="E285" s="11" t="s">
         <v>13</v>
       </c>
@@ -4483,7 +4482,7 @@
       <c r="C286" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D286" s="27"/>
+      <c r="D286" s="26"/>
     </row>
     <row r="287" spans="2:9" ht="13.2">
       <c r="B287" s="8" t="s">
@@ -4492,12 +4491,12 @@
       <c r="C287" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D287" s="27"/>
+      <c r="D287" s="26"/>
     </row>
     <row r="288" spans="2:9" ht="13.2">
       <c r="B288" s="6"/>
       <c r="C288" s="6"/>
-      <c r="D288" s="27"/>
+      <c r="D288" s="26"/>
       <c r="I288" s="11" t="s">
         <v>13</v>
       </c>
@@ -4507,7 +4506,7 @@
       <c r="C289" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D289" s="27"/>
+      <c r="D289" s="26"/>
     </row>
     <row r="290" spans="2:9" ht="13.2">
       <c r="B290" s="8" t="s">
@@ -4516,7 +4515,7 @@
       <c r="C290" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D290" s="27"/>
+      <c r="D290" s="26"/>
       <c r="H290" s="11" t="s">
         <v>13</v>
       </c>
@@ -4528,7 +4527,7 @@
       <c r="C291" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D291" s="27"/>
+      <c r="D291" s="26"/>
     </row>
     <row r="292" spans="2:9" ht="13.2">
       <c r="B292" s="8" t="s">
@@ -4537,24 +4536,24 @@
       <c r="C292" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D292" s="27"/>
+      <c r="D292" s="26"/>
     </row>
     <row r="293" spans="2:9" ht="13.2">
       <c r="B293" s="6"/>
       <c r="C293" s="6"/>
-      <c r="D293" s="27"/>
+      <c r="D293" s="26"/>
     </row>
     <row r="294" spans="2:9" ht="13.2">
       <c r="B294" s="6"/>
       <c r="C294" s="6"/>
-      <c r="D294" s="27"/>
+      <c r="D294" s="26"/>
     </row>
     <row r="295" spans="2:9" ht="13.2">
       <c r="B295" s="6"/>
       <c r="C295" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D295" s="27"/>
+      <c r="D295" s="26"/>
     </row>
     <row r="296" spans="2:9" ht="13.2">
       <c r="B296" s="8" t="s">
@@ -4563,7 +4562,7 @@
       <c r="C296" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D296" s="27"/>
+      <c r="D296" s="26"/>
     </row>
     <row r="297" spans="2:9" ht="13.2">
       <c r="B297" s="8" t="s">
@@ -4572,7 +4571,7 @@
       <c r="C297" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="D297" s="27"/>
+      <c r="D297" s="26"/>
     </row>
     <row r="298" spans="2:9" ht="13.2">
       <c r="B298" s="8" t="s">
@@ -4581,7 +4580,7 @@
       <c r="C298" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D298" s="27"/>
+      <c r="D298" s="26"/>
       <c r="I298" s="11" t="s">
         <v>13</v>
       </c>
@@ -4593,7 +4592,7 @@
       <c r="C299" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="D299" s="27"/>
+      <c r="D299" s="26"/>
     </row>
     <row r="300" spans="2:9" ht="13.2">
       <c r="B300" s="8" t="s">
@@ -4602,7 +4601,7 @@
       <c r="C300" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D300" s="27"/>
+      <c r="D300" s="26"/>
       <c r="H300" s="11" t="s">
         <v>13</v>
       </c>
@@ -4614,7 +4613,7 @@
       <c r="C301" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="D301" s="27"/>
+      <c r="D301" s="26"/>
       <c r="H301" s="11" t="s">
         <v>13</v>
       </c>
@@ -4626,7 +4625,7 @@
       <c r="C302" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="D302" s="27"/>
+      <c r="D302" s="26"/>
       <c r="H302" s="11" t="s">
         <v>13</v>
       </c>
@@ -4638,7 +4637,7 @@
       <c r="C303" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="D303" s="27"/>
+      <c r="D303" s="26"/>
       <c r="H303" s="11" t="s">
         <v>13</v>
       </c>
@@ -4650,7 +4649,7 @@
       <c r="C304" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="D304" s="27"/>
+      <c r="D304" s="26"/>
     </row>
     <row r="305" spans="2:9" ht="13.2">
       <c r="B305" s="8" t="s">
@@ -4659,12 +4658,12 @@
       <c r="C305" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="D305" s="27"/>
+      <c r="D305" s="26"/>
     </row>
     <row r="306" spans="2:9" ht="13.2">
       <c r="B306" s="6"/>
       <c r="C306" s="6"/>
-      <c r="D306" s="27"/>
+      <c r="D306" s="26"/>
       <c r="I306" s="11" t="s">
         <v>13</v>
       </c>
@@ -4672,14 +4671,14 @@
     <row r="307" spans="2:9" ht="13.2">
       <c r="B307" s="6"/>
       <c r="C307" s="6"/>
-      <c r="D307" s="27"/>
+      <c r="D307" s="26"/>
     </row>
     <row r="308" spans="2:9" ht="13.2">
       <c r="B308" s="6"/>
-      <c r="C308" s="25" t="s">
+      <c r="C308" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="D308" s="27"/>
+      <c r="D308" s="26"/>
     </row>
     <row r="309" spans="2:9" ht="13.2">
       <c r="B309" s="8" t="s">
@@ -4688,7 +4687,7 @@
       <c r="C309" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D309" s="27"/>
+      <c r="D309" s="26"/>
     </row>
     <row r="310" spans="2:9" ht="13.2">
       <c r="B310" s="8" t="s">
@@ -4697,7 +4696,7 @@
       <c r="C310" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="D310" s="27"/>
+      <c r="D310" s="26"/>
     </row>
     <row r="311" spans="2:9" ht="13.2">
       <c r="B311" s="8" t="s">
@@ -4706,7 +4705,7 @@
       <c r="C311" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D311" s="28" t="s">
+      <c r="D311" s="27" t="s">
         <v>13</v>
       </c>
       <c r="I311" s="11" t="s">
@@ -4720,7 +4719,7 @@
       <c r="C312" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="D312" s="27"/>
+      <c r="D312" s="26"/>
     </row>
     <row r="313" spans="2:9" ht="13.2">
       <c r="B313" s="8" t="s">
@@ -4729,7 +4728,7 @@
       <c r="C313" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="D313" s="27"/>
+      <c r="D313" s="26"/>
     </row>
     <row r="314" spans="2:9" ht="13.2">
       <c r="B314" s="8" t="s">
@@ -4738,7 +4737,7 @@
       <c r="C314" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="D314" s="27"/>
+      <c r="D314" s="26"/>
     </row>
     <row r="315" spans="2:9" ht="13.2">
       <c r="B315" s="8" t="s">
@@ -4747,7 +4746,7 @@
       <c r="C315" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D315" s="27"/>
+      <c r="D315" s="26"/>
       <c r="H315" s="11" t="s">
         <v>13</v>
       </c>
@@ -4759,7 +4758,7 @@
       <c r="C316" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D316" s="27"/>
+      <c r="D316" s="26"/>
     </row>
     <row r="317" spans="2:9" ht="13.2">
       <c r="B317" s="8" t="s">
@@ -4768,7 +4767,7 @@
       <c r="C317" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D317" s="28" t="s">
+      <c r="D317" s="27" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4779,7 +4778,7 @@
       <c r="C318" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D318" s="27"/>
+      <c r="D318" s="26"/>
       <c r="F318" s="11" t="s">
         <v>13</v>
       </c>
@@ -4791,7 +4790,7 @@
       <c r="C319" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="D319" s="27"/>
+      <c r="D319" s="26"/>
     </row>
     <row r="320" spans="2:9" ht="13.2">
       <c r="B320" s="8" t="s">
@@ -4800,7 +4799,7 @@
       <c r="C320" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="D320" s="27"/>
+      <c r="D320" s="26"/>
       <c r="H320" s="11" t="s">
         <v>13</v>
       </c>
@@ -4812,7 +4811,7 @@
       <c r="C321" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="D321" s="27"/>
+      <c r="D321" s="26"/>
       <c r="H321" s="11"/>
     </row>
     <row r="322" spans="2:8" ht="13.2">
@@ -4822,7 +4821,7 @@
       <c r="C322" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="D322" s="27"/>
+      <c r="D322" s="26"/>
       <c r="H322" s="11" t="s">
         <v>13</v>
       </c>
@@ -4834,7 +4833,7 @@
       <c r="C323" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="D323" s="27"/>
+      <c r="D323" s="26"/>
       <c r="H323" s="11" t="s">
         <v>13</v>
       </c>
@@ -4846,7 +4845,7 @@
       <c r="C324" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="D324" s="27"/>
+      <c r="D324" s="26"/>
       <c r="E324" s="11" t="s">
         <v>13</v>
       </c>
@@ -4858,7 +4857,7 @@
       <c r="C325" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="D325" s="27"/>
+      <c r="D325" s="26"/>
     </row>
     <row r="326" spans="2:8" ht="13.2">
       <c r="B326" s="8" t="s">
@@ -4867,19 +4866,19 @@
       <c r="C326" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="D326" s="27"/>
+      <c r="D326" s="26"/>
     </row>
     <row r="327" spans="2:8" ht="13.2">
       <c r="B327" s="6"/>
       <c r="C327" s="6"/>
-      <c r="D327" s="27"/>
+      <c r="D327" s="26"/>
     </row>
     <row r="328" spans="2:8" ht="13.8">
       <c r="B328" s="6"/>
-      <c r="C328" s="26" t="s">
+      <c r="C328" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="D328" s="27"/>
+      <c r="D328" s="26"/>
     </row>
     <row r="329" spans="2:8" ht="13.2">
       <c r="B329" s="8" t="s">
@@ -4888,7 +4887,7 @@
       <c r="C329" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="D329" s="28" t="s">
+      <c r="D329" s="27" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4899,7 +4898,7 @@
       <c r="C330" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="D330" s="27"/>
+      <c r="D330" s="26"/>
       <c r="G330" s="11" t="s">
         <v>13</v>
       </c>
@@ -4911,7 +4910,7 @@
       <c r="C331" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D331" s="27"/>
+      <c r="D331" s="26"/>
     </row>
     <row r="332" spans="2:8" ht="13.2">
       <c r="B332" s="8" t="s">
@@ -4920,13 +4919,13 @@
       <c r="C332" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="D332" s="27"/>
+      <c r="D332" s="26"/>
       <c r="H332" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="333" spans="2:8" ht="13.2">
-      <c r="D333" s="27"/>
+      <c r="D333" s="26"/>
       <c r="E333" s="11" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
2 sorting easy question solved
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2469A5C-F688-48E6-8908-5E5AE0BBC17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE2C5A5-7C77-4EC1-8EF8-2FAE4585969B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2329,7 +2329,7 @@
       <c r="C80" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="26"/>
+      <c r="D80" s="28"/>
       <c r="G80" s="10" t="s">
         <v>13</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="C81" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="26"/>
+      <c r="D81" s="28"/>
     </row>
     <row r="82" spans="2:9" ht="15">
       <c r="B82" s="8" t="s">

</xml_diff>

<commit_message>
solved searching and sorting problems
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE2C5A5-7C77-4EC1-8EF8-2FAE4585969B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCA27F0-2F49-4250-9F3F-AF8A36B469C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2162,7 +2162,7 @@
       <c r="C62" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="26"/>
+      <c r="D62" s="28"/>
       <c r="H62" s="11" t="s">
         <v>13</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="C63" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="26"/>
+      <c r="D63" s="28"/>
       <c r="H63" s="10" t="s">
         <v>13</v>
       </c>
@@ -2350,7 +2350,7 @@
       <c r="C82" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D82" s="26"/>
+      <c r="D82" s="28"/>
       <c r="F82" s="10" t="s">
         <v>13</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="C83" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D83" s="26"/>
+      <c r="D83" s="28"/>
     </row>
     <row r="84" spans="2:9" ht="15">
       <c r="B84" s="8" t="s">
@@ -2383,7 +2383,7 @@
       <c r="C85" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D85" s="26"/>
+      <c r="D85" s="28"/>
       <c r="E85" s="5" t="s">
         <v>13</v>
       </c>
@@ -2395,7 +2395,7 @@
       <c r="C86" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D86" s="26"/>
+      <c r="D86" s="28"/>
     </row>
     <row r="87" spans="2:9" ht="15">
       <c r="B87" s="8" t="s">

</xml_diff>

<commit_message>
3 linked list question solved
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCA27F0-2F49-4250-9F3F-AF8A36B469C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870F8C1B-334F-4F75-B0BB-88F18184597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2501,7 +2501,7 @@
       <c r="C97" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D97" s="26"/>
+      <c r="D97" s="28"/>
     </row>
     <row r="98" spans="2:9" ht="13.2">
       <c r="B98" s="8" t="s">
@@ -2522,7 +2522,7 @@
       <c r="C99" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D99" s="26"/>
+      <c r="D99" s="28"/>
       <c r="I99" s="10" t="s">
         <v>13</v>
       </c>
@@ -2534,7 +2534,7 @@
       <c r="C100" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D100" s="26"/>
+      <c r="D100" s="28"/>
     </row>
     <row r="101" spans="2:9" ht="13.2">
       <c r="B101" s="8" t="s">

</xml_diff>

<commit_message>
solved a medium linked list problem
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE1780C-CA6D-4737-90C0-B77A0715CB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB85EC-3EC7-4E0F-95C6-E5A218C6F437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2655,7 +2655,7 @@
       <c r="C111" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D111" s="26"/>
+      <c r="D111" s="28"/>
     </row>
     <row r="112" spans="2:9" ht="13.2">
       <c r="B112" s="8" t="s">

</xml_diff>

<commit_message>
valid pallindrome II added
</commit_message>
<xml_diff>
--- a/#DSASheetbyArsh (45-60 Days).xlsx
+++ b/#DSASheetbyArsh (45-60 Days).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subha\Documents\Shubham-CrackYourInternship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D645D3A1-4565-46A0-B807-6453A827F6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B31BD1-FCE5-41D3-BC6A-B423D2797F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:I333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1943,7 +1943,7 @@
       <c r="C41" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="26"/>
+      <c r="D41" s="28"/>
       <c r="E41" s="10" t="s">
         <v>13</v>
       </c>

</xml_diff>